<commit_message>
Commit function: read excel + open browser
</commit_message>
<xml_diff>
--- a/Test_Input/TestCase.xlsx
+++ b/Test_Input/TestCase.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8805" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8805" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="TC2" sheetId="4" r:id="rId2"/>
+    <sheet name="Register" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="4" r:id="rId2"/>
     <sheet name="TestConfig" sheetId="2" r:id="rId3"/>
     <sheet name="ConfigData" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ConfigData!$A$1:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ConfigData!$A$1:$D$7</definedName>
     <definedName name="RunningOption">ConfigData!$A$1:$A$2</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Sheet</t>
   </si>
@@ -77,15 +77,6 @@
     <t>Run IE</t>
   </si>
   <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Login with valid data</t>
-  </si>
-  <si>
     <t>Result FF</t>
   </si>
   <si>
@@ -132,13 +123,31 @@
   </si>
   <si>
     <t>Wait page load</t>
+  </si>
+  <si>
+    <t>http://newtours.demoaut.com/mercuryunderconst.php</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Register with valid data</t>
+  </si>
+  <si>
+    <t>//a[contains(text(),'REGISTER')]</t>
+  </si>
+  <si>
+    <t>Register: Mercury Tours</t>
+  </si>
+  <si>
+    <t>AssertPageTitle(Expected output)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +170,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -226,7 +241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -253,15 +268,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -323,7 +342,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,7 +377,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -567,19 +586,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="13" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
@@ -608,13 +630,13 @@
         <v>9</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>10</v>
@@ -625,66 +647,74 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>33</v>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>26</v>
+      <c r="A8" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -692,12 +722,18 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ConfigData!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C6 C9</xm:sqref>
+          <xm:sqref>C6:C7 C10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>ConfigData!$D$2:$D$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3:B7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -709,50 +745,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="13" width="17.5703125" style="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:13" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="16" t="s">
+      <c r="I1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="15" t="s">
         <v>11</v>
       </c>
     </row>
@@ -763,10 +802,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,13 +837,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -816,32 +855,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
       <formula1>RunningOption+RunningOption</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:D3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:D2">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -852,11 +871,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,48 +886,53 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D6" s="13" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D6"/>
+  <autoFilter ref="A1:D7"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
complete ClickKeyWords and AssertKeyWords.java and Quit
</commit_message>
<xml_diff>
--- a/Test_Input/TestCase.xlsx
+++ b/Test_Input/TestCase.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
   <si>
     <t>Sheet</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Register with invalid data</t>
+  </si>
+  <si>
+    <t>Click on Button(Find Element By, By Value)</t>
+  </si>
+  <si>
+    <t>Assert PageTitle(Expected output)</t>
   </si>
 </sst>
 </file>
@@ -238,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -259,7 +265,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -583,7 +588,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -653,22 +658,22 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
-        <v>22</v>
+      <c r="B6" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -677,57 +682,65 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+    <row r="7" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="18" t="s">
+    </row>
+    <row r="14" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H13" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -735,13 +748,13 @@
           <x14:formula1>
             <xm:f>ConfigData!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C6:C7 C11:C13</xm:sqref>
+          <xm:sqref>C6:C8 C12:C14</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>ConfigData!$D$2:$D$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:B13</xm:sqref>
+          <xm:sqref>B3:B14</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -759,47 +772,47 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="13" width="17.5703125" style="17" customWidth="1"/>
+    <col min="1" max="13" width="17.5703125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:13" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="14" t="s">
         <v>10</v>
       </c>
     </row>
@@ -813,7 +826,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,13 +861,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -870,10 +883,10 @@
       <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E3">
@@ -903,7 +916,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,7 +937,7 @@
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -932,7 +945,7 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -940,22 +953,22 @@
       <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>22</v>
+      <c r="D4" s="10" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="13" t="s">
-        <v>35</v>
+    <row r="6" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>